<commit_message>
Test por nombre de producto
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/Data.xlsx
+++ b/src/main/resources/Data/Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>Search</t>
   </si>
@@ -87,6 +87,21 @@
   </si>
   <si>
     <t>KOORUI Monitor de juegos de 24 pulgadas, monitor de computadora FHD 1080P de 165 Hz VA 1 ms integrado FreeSync, compatible con G-sync, monitores LED con ultrafino, compatible con HDMI X2/DP, VESA, cuidado de los ojos 24E4, negro</t>
+  </si>
+  <si>
+    <t>Acer Nitro KG241Y Sbiip Monitor para juegos VA Full HD (1920 x 1080) de 23.8 pulgadas | Tecnología AMD FreeSync Premium | Frecuencia de actualización de 165 Hz | 1 ms (VRB) | Diseño ZeroFrame | 1 puerto de pantalla 1.2 y 2 x HDMI 2.0</t>
+  </si>
+  <si>
+    <t>KOORUI Monitor de computadora de 27 pulgadas, FHD 1920 x 1080p, monitor IPS de 75 Hz, HDMI, VGA, montaje VESA de 2.953 x 2.953 in, sin marco, protección ocular y ajuste ergonómico de inclinación</t>
+  </si>
+  <si>
+    <t>KOORUI Monitor de juegos de 27 pulgadas, QHD (2560 x 1440), monitores de computadora giratorios verticales, 144 Hz/170Hz, IPS, 1 ms, HDR 400, sincronización adpitiva, 2 monitores HDMI y DisplayPort 2K, altura ajustable</t>
+  </si>
+  <si>
+    <t>KOORUI 24 Inch Curved Computer Monitor, 60Hz 1080p FHD Desktop Monitor VA Panel with HDMI VGA Ports Free Flicker Low BlueLight, sRGB 99% Led Monitor for PC Home Office, VESA Compatible Black (24N5C)</t>
+  </si>
+  <si>
+    <t>KOORUI Monitor curvo ultra ancho de 34 pulgadas para juegos 165HZ, 1ms, 1000R, WQHD 3440 x 1440, 21:9, DCI-P3 90% de gama de colores, compatible con FreeSync G-Sync, soporte ajustable de inclinación/altura, HDMI, puerto de pantalla, negro</t>
   </si>
 </sst>
 </file>
@@ -455,7 +470,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test con validacion de titulo y cantidad
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/Data.xlsx
+++ b/src/main/resources/Data/Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>Search</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>KOORUI Monitor curvo ultra ancho de 34 pulgadas para juegos 165HZ, 1ms, 1000R, WQHD 3440 x 1440, 21:9, DCI-P3 90% de gama de colores, compatible con FreeSync G-Sync, soporte ajustable de inclinación/altura, HDMI, puerto de pantalla, negro</t>
+  </si>
+  <si>
+    <t>KOORUI Monitor de computadora de 22 pulgadas, pantalla de escritorio FHD 1080P, bisel ultrafino/cuidado de los ojos/inclinación ergonómica, puertos HDMI VGA</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>